<commit_message>
Add note on motor calibration
</commit_message>
<xml_diff>
--- a/Motor_Calibration/Data_500 samples/MDP_Motor2.xlsx
+++ b/Motor_Calibration/Data_500 samples/MDP_Motor2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Boom\Documents\MDP2019\Motor_Calibration\Data_500 samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Boom\Documents\MDP2019\CE3004---Mdp-Group-14-Arduino\Motor_Calibration\Data_500 samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EFE9E35-C62E-4830-A91D-6A3DB66ACBF6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96809B34-FF90-43F2-A55C-64B8103B9C7B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="612" windowWidth="17280" windowHeight="9060" activeTab="2" xr2:uid="{224FD1F9-9E51-4E69-A005-FB6DA346CC02}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{224FD1F9-9E51-4E69-A005-FB6DA346CC02}"/>
   </bookViews>
   <sheets>
     <sheet name="Motor1A" sheetId="1" r:id="rId1"/>
@@ -222,7 +222,9 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -288,138 +290,102 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Overall!$D$28:$D$47</c:f>
+              <c:f>Overall!$D$30:$D$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>130.86333310616902</c:v>
+                  <c:v>119.63356715009679</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>127.71782590049578</c:v>
+                  <c:v>111.76348945799792</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>119.63356715009679</c:v>
+                  <c:v>103.41750759071887</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>111.76348945799792</c:v>
+                  <c:v>95.609320205401247</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.41750759071887</c:v>
+                  <c:v>87.428029218046802</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95.609320205401247</c:v>
+                  <c:v>79.720105251342375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87.428029218046802</c:v>
+                  <c:v>72.023269570617074</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79.720105251342375</c:v>
+                  <c:v>64.825160902204743</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.023269570617074</c:v>
+                  <c:v>57.46018556890931</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>64.825160902204743</c:v>
+                  <c:v>50.440634402342233</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>57.46018556890931</c:v>
+                  <c:v>43.796355514193877</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50.440634402342233</c:v>
+                  <c:v>36.962540841283662</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43.796355514193877</c:v>
+                  <c:v>30.295107904938309</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.962540841283662</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30.295107904938309</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>23.888942495365647</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17.890268130227291</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12.269713194739154</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.3021068602129295</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.1932330387904067</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Overall!$F$28:$F$47</c:f>
+              <c:f>Overall!$F$30:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>380</c:v>
+                  <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>360</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>340</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>320</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>300</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>280</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>260</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>240</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>220</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>200</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>180</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>160</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -691,7 +657,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -709,7 +675,9 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -773,145 +741,153 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.7475940507436569E-4"/>
+                  <c:y val="0.14034230096237965"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Overall!$E$28:$E$47</c:f>
+              <c:f>Overall!$E$31:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>133.04807214138577</c:v>
+                  <c:v>115.27027221145582</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130.39826437485715</c:v>
+                  <c:v>107.17095940264787</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>123.31096499585105</c:v>
+                  <c:v>99.424423200572292</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>115.27027221145582</c:v>
+                  <c:v>91.22882063828537</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>107.17095940264787</c:v>
+                  <c:v>82.673294104132481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99.424423200572292</c:v>
+                  <c:v>75.604073250773482</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>91.22882063828537</c:v>
+                  <c:v>67.786188502652905</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>82.673294104132481</c:v>
+                  <c:v>60.63149886140959</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75.604073250773482</c:v>
+                  <c:v>53.852771997820135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>67.786188502652905</c:v>
+                  <c:v>46.708770539650715</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60.63149886140959</c:v>
+                  <c:v>39.497803395297133</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53.852771997820135</c:v>
+                  <c:v>32.570905548865383</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46.708770539650715</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>39.497803395297133</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32.570905548865383</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>26.271086450579485</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>20.298613085804195</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>14.614413106261566</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.722801130464342</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.3748717263195775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Overall!$F$28:$F$47</c:f>
+              <c:f>Overall!$F$31:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>380</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>360</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>340</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>320</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>300</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>280</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>260</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>240</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>220</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>200</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>180</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-28B7-4C0A-BDEC-D9C4F3536D60}"/>
@@ -37051,15 +37027,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D7371F-D93B-4366-BF24-210236153428}">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
@@ -72387,6 +72364,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFEFB9236B204D4A9CEFB6E5EB7278E6" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b2767b0c44aa1648a4e25ce7293d33a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e5742000-0468-4752-8afa-b2d1c3eb18ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6906b666629a79a52cb6fdb8b79fdc78" ns3:_="">
     <xsd:import namespace="e5742000-0468-4752-8afa-b2d1c3eb18ef"/>
@@ -72548,22 +72540,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7924EC85-7689-4B66-BAE2-621D77E5E7F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e5742000-0468-4752-8afa-b2d1c3eb18ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40468622-DC4E-47EF-923E-ADD319BA63A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49CBD21B-7951-4464-BE9F-85BC92EB9EE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -72579,28 +72580,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40468622-DC4E-47EF-923E-ADD319BA63A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7924EC85-7689-4B66-BAE2-621D77E5E7F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e5742000-0468-4752-8afa-b2d1c3eb18ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>